<commit_message>
Made some changes.. and improving all over code quality...
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -23,7 +23,7 @@
     <t>Author</t>
   </si>
   <si>
-    <t>Code</t>
+    <t>Book Code</t>
   </si>
   <si>
     <t>No</t>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>hi</t>
-  </si>
-  <si>
-    <t>hi]</t>
   </si>
 </sst>
 </file>
@@ -443,7 +440,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -451,16 +448,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed a lot of bugs and improved all over working of the program..
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -33,12 +33,6 @@
   </si>
   <si>
     <t>hello</t>
-  </si>
-  <si>
-    <t>hel</t>
-  </si>
-  <si>
-    <t>hi</t>
   </si>
 </sst>
 </file>
@@ -387,7 +381,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,30 +428,13 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now in a nearly working condition.. reissuing not looked upon..
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -32,7 +32,13 @@
     <t>test</t>
   </si>
   <si>
-    <t>hello</t>
+    <t>Python Fundamentals</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>T112</t>
   </si>
 </sst>
 </file>
@@ -428,13 +434,13 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>